<commit_message>
bugfix allow duplicate column names + tests
</commit_message>
<xml_diff>
--- a/tests/MiscTableToDicts/MiscTableToDicts.xlsx
+++ b/tests/MiscTableToDicts/MiscTableToDicts.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa\MiscVBAFunctions\tests\MiscTableToDicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC120059-B1B2-49A1-850A-F8B36A35B3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9D227C-C3D4-47C1-982E-0357A4E03C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{70234706-DE99-425E-A585-1A07C6E034F2}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{70234706-DE99-425E-A585-1A07C6E034F2}"/>
   </bookViews>
   <sheets>
     <sheet name="TableToDicts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="NamedRange1">TableToDicts!$G$4:$I$6</definedName>
-    <definedName name="NamedRange2">TableToDicts!$Q$4:$S$4</definedName>
-    <definedName name="NamedRange3">TableToDicts!$Y$4</definedName>
+    <definedName name="NamedRange1">TableToDicts!$G$4:$L$6</definedName>
+    <definedName name="NamedRange2">TableToDicts!$T$4:$V$4</definedName>
+    <definedName name="NamedRange3">TableToDicts!$AB$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>c</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>ListObject3</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Case insensitive and uses last instance of c</t>
   </si>
 </sst>
 </file>
@@ -81,12 +87,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -133,8 +146,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{14C84F34-9841-4F98-BB90-5BB01ED90D88}" name="ListObject2" displayName="ListObject2" ref="L4:N5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="L4:N5" xr:uid="{14C84F34-9841-4F98-BB90-5BB01ED90D88}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{14C84F34-9841-4F98-BB90-5BB01ED90D88}" name="ListObject2" displayName="ListObject2" ref="O4:Q5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="O4:Q5" xr:uid="{14C84F34-9841-4F98-BB90-5BB01ED90D88}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A51123E8-F61C-4B77-B669-B6442FCD071D}" name="a"/>
     <tableColumn id="2" xr3:uid="{30138679-3458-4E22-88F0-F9DD48840A97}" name="b"/>
@@ -145,8 +158,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{55378EA3-D06B-4736-9F00-AF1867DFF68D}" name="ListObject3" displayName="ListObject3" ref="V4:V5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="V4:V5" xr:uid="{55378EA3-D06B-4736-9F00-AF1867DFF68D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{55378EA3-D06B-4736-9F00-AF1867DFF68D}" name="ListObject3" displayName="ListObject3" ref="Y4:Y5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="Y4:Y5" xr:uid="{55378EA3-D06B-4736-9F00-AF1867DFF68D}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{84024F07-52F4-4E3B-A167-6B25498492E4}" name="a"/>
   </tableColumns>
@@ -452,35 +465,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA4CCA1-6978-4BBA-979B-493FFE6B4701}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:Y6"/>
+  <dimension ref="B2:AB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>6</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AB2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -490,41 +508,46 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" t="s">
         <v>1</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>0</v>
       </c>
-      <c r="Q4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" t="s">
         <v>1</v>
       </c>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>0</v>
       </c>
-      <c r="V4" t="s">
-        <v>2</v>
-      </c>
       <c r="Y4" t="s">
         <v>2</v>
       </c>
+      <c r="AB4" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -534,17 +557,22 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -554,13 +582,18 @@
       <c r="D6">
         <v>6</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1">
         <v>5</v>
       </c>
-      <c r="I6">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <v>60</v>
+      </c>
+      <c r="L6" s="1">
         <v>6</v>
       </c>
     </row>

</xml_diff>